<commit_message>
Added 2-D images to wavelets.Rmd
</commit_message>
<xml_diff>
--- a/text/14/wavelets-03.xlsx
+++ b/text/14/wavelets-03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\git\blogdown-backup\text\14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736703EB-3750-465E-8FE8-410182EE4FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AF0E27-5A24-4EE5-900C-97D997F5F26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{52B52DA5-282C-469E-8823-90CEECEA51FB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="21">
   <si>
     <t>⋮</t>
   </si>
@@ -328,6 +328,9 @@
       </rPr>
       <t>k3</t>
     </r>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -504,6 +507,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -820,61 +826,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3B9B88-5760-4CC4-AAA3-89D7B6C5F7A6}">
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:AG27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AH17" sqref="AH17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.88671875" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.88671875" style="3"/>
     <col min="2" max="2" width="1.109375" style="1" customWidth="1"/>
-    <col min="3" max="15" width="3.33203125" style="1" customWidth="1"/>
+    <col min="3" max="11" width="3.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="1.109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="1.109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="1.109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="3.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="1.109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="4.88671875" style="3"/>
     <col min="18" max="18" width="1.109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="3.33203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="1.109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="4.88671875" style="3"/>
-    <col min="22" max="16384" width="4.88671875" style="1"/>
+    <col min="19" max="27" width="3.33203125" style="1" customWidth="1"/>
+    <col min="28" max="30" width="1.109375" style="1" customWidth="1"/>
+    <col min="31" max="31" width="3.33203125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="1.109375" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="4.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="1:20" ht="6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:33" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="AC1" s="3"/>
+      <c r="AG1" s="3"/>
+    </row>
+    <row r="2" spans="1:33" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="9"/>
+      <c r="L2" s="10"/>
+      <c r="N2" s="9"/>
       <c r="P2" s="10"/>
       <c r="R2" s="9"/>
-      <c r="T2" s="10"/>
-    </row>
-    <row r="3" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="9"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="3"/>
+    </row>
+    <row r="3" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5"/>
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="M3" s="1" t="s">
+      <c r="G3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="K3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="6"/>
+      <c r="N3" s="5"/>
       <c r="O3" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P3" s="6"/>
       <c r="R3" s="5"/>
       <c r="S3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T3" s="6"/>
-    </row>
-    <row r="4" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="3"/>
+    </row>
+    <row r="4" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -884,27 +926,49 @@
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="N4" s="1" t="s">
+      <c r="G4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="L4" s="6"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="1">
+        <v>0</v>
       </c>
       <c r="P4" s="6"/>
       <c r="R4" s="5"/>
-      <c r="S4" s="1">
+      <c r="S4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="1">
         <v>0</v>
       </c>
-      <c r="T4" s="6"/>
-    </row>
-    <row r="5" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="3"/>
+    </row>
+    <row r="5" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -915,22 +979,44 @@
       <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="N5" s="5"/>
       <c r="O5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P5" s="6"/>
       <c r="R5" s="5"/>
       <c r="S5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T5" s="6"/>
-    </row>
-    <row r="6" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+        <v>12</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="3"/>
+    </row>
+    <row r="6" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -944,21 +1030,41 @@
       <c r="F6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
       <c r="P6" s="6"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="1">
+      <c r="S6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="1">
         <v>0</v>
       </c>
-      <c r="T6" s="6"/>
-    </row>
-    <row r="7" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="3"/>
+    </row>
+    <row r="7" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="5"/>
       <c r="D7" s="1" t="s">
         <v>5</v>
@@ -969,22 +1075,38 @@
       <c r="F7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="6"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="P7" s="6"/>
       <c r="R7" s="5"/>
-      <c r="S7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T7" s="6"/>
-    </row>
-    <row r="8" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="T7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="3"/>
+    </row>
+    <row r="8" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="5"/>
       <c r="E8" s="1" t="s">
         <v>5</v>
@@ -992,378 +1114,207 @@
       <c r="F8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
       <c r="P8" s="6"/>
+      <c r="Q8" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="R8" s="5"/>
-      <c r="S8" s="1">
+      <c r="U8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="W8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="1">
         <v>0</v>
       </c>
-      <c r="T8" s="6"/>
-    </row>
-    <row r="9" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="3"/>
+    </row>
+    <row r="9" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="5"/>
-      <c r="I9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="L9" s="6"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="P9" s="6"/>
       <c r="R9" s="5"/>
-      <c r="S9" s="4" t="s">
+      <c r="W9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="T9" s="6"/>
-    </row>
-    <row r="10" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="3"/>
+    </row>
+    <row r="10" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="5"/>
-      <c r="I10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L10" s="1" t="s">
+      <c r="G10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="P10" s="6"/>
       <c r="R10" s="5"/>
-      <c r="S10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="T10" s="6"/>
-    </row>
-    <row r="11" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="W10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="3"/>
+    </row>
+    <row r="11" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="I11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L11" s="1" t="s">
+      <c r="G11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="L11" s="6"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="1">
+        <v>0</v>
       </c>
       <c r="P11" s="6"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="1">
+      <c r="W11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="1">
         <v>0</v>
       </c>
-      <c r="T11" s="6"/>
-    </row>
-    <row r="12" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="3"/>
+    </row>
+    <row r="12" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="5"/>
-      <c r="I12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1" t="s">
+      <c r="G12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="K12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="6"/>
+      <c r="N12" s="5"/>
       <c r="O12" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P12" s="6"/>
       <c r="R12" s="5"/>
-      <c r="S12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T12" s="6"/>
-    </row>
-    <row r="13" spans="1:20" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="W12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF12" s="6"/>
+      <c r="AG12" s="3"/>
+    </row>
+    <row r="13" spans="1:33" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B13" s="8"/>
+      <c r="L13" s="7"/>
+      <c r="N13" s="8"/>
       <c r="P13" s="7"/>
       <c r="R13" s="8"/>
-      <c r="T13" s="7"/>
-    </row>
-    <row r="15" spans="1:20" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="16" spans="1:20" ht="6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="8"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="3"/>
+    </row>
+    <row r="14" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AC14" s="3"/>
+      <c r="AG14" s="3"/>
+    </row>
+    <row r="16" spans="1:33" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2"/>
-      <c r="B16" s="9"/>
-      <c r="P16" s="10"/>
-      <c r="R16" s="9"/>
-      <c r="T16" s="10"/>
-    </row>
-    <row r="17" spans="2:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="5"/>
-      <c r="C17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="M17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P17" s="6"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T17" s="6"/>
-    </row>
-    <row r="18" spans="2:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="5"/>
-      <c r="C18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="N18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P18" s="6"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="1">
-        <v>0</v>
-      </c>
-      <c r="T18" s="6"/>
-    </row>
-    <row r="19" spans="2:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="5"/>
-      <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="O19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P19" s="6"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T19" s="6"/>
-    </row>
-    <row r="20" spans="2:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="5"/>
-      <c r="C20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="P20" s="6"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="1">
-        <v>0</v>
-      </c>
-      <c r="T20" s="6"/>
-    </row>
-    <row r="21" spans="2:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="5"/>
-      <c r="D21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="P21" s="6"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T21" s="6"/>
-    </row>
-    <row r="22" spans="2:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="5"/>
-      <c r="E22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="P22" s="6"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="1">
-        <v>0</v>
-      </c>
-      <c r="T22" s="6"/>
-    </row>
-    <row r="23" spans="2:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="5"/>
-      <c r="I23" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="P23" s="6"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="T23" s="6"/>
-    </row>
-    <row r="24" spans="2:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="5"/>
-      <c r="I24" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P24" s="6"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T24" s="6"/>
-    </row>
-    <row r="25" spans="2:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="5"/>
-      <c r="I25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P25" s="6"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="1">
-        <v>0</v>
-      </c>
-      <c r="T25" s="6"/>
-    </row>
-    <row r="26" spans="2:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="5"/>
-      <c r="I26" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P26" s="6"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T26" s="6"/>
-    </row>
-    <row r="27" spans="2:20" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="8"/>
-      <c r="P27" s="7"/>
-      <c r="R27" s="8"/>
-      <c r="T27" s="7"/>
-    </row>
+    </row>
+    <row r="27" ht="6" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>